<commit_message>
Added Return Data and Invoice Data
</commit_message>
<xml_diff>
--- a/data-pipeline-app/documentation/docs/Capstone Supplier Performance Analysis Data Guide.xlsx
+++ b/data-pipeline-app/documentation/docs/Capstone Supplier Performance Analysis Data Guide.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHAKTI_GOYAL\capstone-project\data-eng-capstone-project-teameinstein\data-pipeline-app\documentation\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parvathi_Gokavarapu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC64CD6-4069-47C2-BF9F-2AAE821FE453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36210CE6-378F-4175-967D-8AB0A77D0EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="893" firstSheet="1" activeTab="10" xr2:uid="{C47A438E-1665-47B3-8C39-BF484954AF81}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="893" firstSheet="2" activeTab="12" xr2:uid="{C47A438E-1665-47B3-8C39-BF484954AF81}"/>
   </bookViews>
   <sheets>
     <sheet name="User Guide" sheetId="7" r:id="rId1"/>
@@ -24,9 +24,11 @@
     <sheet name="Compliance Data" sheetId="25" r:id="rId9"/>
     <sheet name="Inventory Management Data" sheetId="10" r:id="rId10"/>
     <sheet name="Perfomance Feedback" sheetId="18" r:id="rId11"/>
+    <sheet name="Return Data" sheetId="26" r:id="rId12"/>
+    <sheet name="Invoice Data" sheetId="27" r:id="rId13"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
     <definedName name="base64binary" localSheetId="2">'Data Types'!$A$9</definedName>
@@ -212,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="348">
   <si>
     <t>Legend</t>
   </si>
@@ -1652,6 +1654,189 @@
   </si>
   <si>
     <t>Hi</t>
+  </si>
+  <si>
+    <t>Return Id</t>
+  </si>
+  <si>
+    <t>return_id</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>R1000</t>
+  </si>
+  <si>
+    <t>Return ID</t>
+  </si>
+  <si>
+    <t>PO Number</t>
+  </si>
+  <si>
+    <t>po_number</t>
+  </si>
+  <si>
+    <t>PO1000</t>
+  </si>
+  <si>
+    <t>supplier_id</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>I1000</t>
+  </si>
+  <si>
+    <t>Return date</t>
+  </si>
+  <si>
+    <t>return_date</t>
+  </si>
+  <si>
+    <t>Return Date</t>
+  </si>
+  <si>
+    <t>Quantity returned</t>
+  </si>
+  <si>
+    <t>qty_returned</t>
+  </si>
+  <si>
+    <t>Reason for return</t>
+  </si>
+  <si>
+    <t>reason_for_return</t>
+  </si>
+  <si>
+    <t>Damaged or defected Item</t>
+  </si>
+  <si>
+    <t>List of reasons of return: Damaged or defected Item, incorrect order, Delivery delay, Misleading product Information</t>
+  </si>
+  <si>
+    <t>Credit issued</t>
+  </si>
+  <si>
+    <t>credit_issued</t>
+  </si>
+  <si>
+    <t>Amount issued as part of credit</t>
+  </si>
+  <si>
+    <t>Return processing time</t>
+  </si>
+  <si>
+    <t>ret_proc_time</t>
+  </si>
+  <si>
+    <t>Return Processing time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foreign Key </t>
+  </si>
+  <si>
+    <t>Invoice ID</t>
+  </si>
+  <si>
+    <t>invoice_id</t>
+  </si>
+  <si>
+    <t>Should Start with INVXXXX. XXXX Integer and the range is 10000 to 11000</t>
+  </si>
+  <si>
+    <t>INV10001,INV10002 etc</t>
+  </si>
+  <si>
+    <t>0..1</t>
+  </si>
+  <si>
+    <t>Should start with POXXXX XXXX Integer and the range is 1000 to 3500</t>
+  </si>
+  <si>
+    <t>PO1000,PO1001 etc</t>
+  </si>
+  <si>
+    <t>random value</t>
+  </si>
+  <si>
+    <t>Should Start with SXXXX. XXXX Integer and the range is 15000 to 16000</t>
+  </si>
+  <si>
+    <t>S15001,S15002 etc</t>
+  </si>
+  <si>
+    <t>Invoice Date</t>
+  </si>
+  <si>
+    <t>invoice_date</t>
+  </si>
+  <si>
+    <t>random date</t>
+  </si>
+  <si>
+    <t>Payment Date</t>
+  </si>
+  <si>
+    <t>payment_date</t>
+  </si>
+  <si>
+    <t>greater than invoice date</t>
+  </si>
+  <si>
+    <t>Payment Terms</t>
+  </si>
+  <si>
+    <t>payment_terms</t>
+  </si>
+  <si>
+    <t>Value should be with in this list</t>
+  </si>
+  <si>
+    <t>NET 30, NET60, NET 90</t>
+  </si>
+  <si>
+    <t>Invoice amount</t>
+  </si>
+  <si>
+    <t>invoice_amount</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>Invoice amount range between 1000 to 5000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paid amount </t>
+  </si>
+  <si>
+    <t>paid_amount</t>
+  </si>
+  <si>
+    <t>should be in the range from 900 and invoice amount</t>
+  </si>
+  <si>
+    <t>Payment Status</t>
+  </si>
+  <si>
+    <t>payment_status</t>
+  </si>
+  <si>
+    <t>comparison between payment date and invoice date</t>
+  </si>
+  <si>
+    <t>On time, Late</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Must be provided </t>
+  </si>
+  <si>
+    <t>Invoice Amount</t>
+  </si>
+  <si>
+    <t>Paid Amount</t>
   </si>
 </sst>
 </file>
@@ -2110,7 +2295,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2257,6 +2442,27 @@
     <xf numFmtId="14" fontId="8" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2281,26 +2487,42 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3072,30 +3294,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1" ht="28.2" x14ac:dyDescent="1.05">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="67" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="60"/>
+      <c r="B1" s="67"/>
     </row>
     <row r="2" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="61"/>
-      <c r="B2" s="61"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
     </row>
     <row r="3" spans="1:3" ht="211" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="69" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="62"/>
+      <c r="B3" s="69"/>
     </row>
     <row r="4" spans="1:3" ht="10.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
     </row>
     <row r="5" spans="1:3" ht="25.8" x14ac:dyDescent="0.95">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="63"/>
+      <c r="B5" s="70"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12" t="s">
@@ -3154,10 +3376,10 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="25.8" x14ac:dyDescent="0.95">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="64"/>
+      <c r="B14" s="71"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="24" t="s">
@@ -3610,11 +3832,11 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3809,6 +4031,719 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D340B162-D877-44CE-8F62-899FE94D2463}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="64.20703125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="18.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.9453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.89453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.1015625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.47265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.62890625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.20703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.47265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="60" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1" s="60" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="75" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>288</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>289</v>
+      </c>
+      <c r="F2" s="63" t="str">
+        <f t="shared" ref="F2:F5" si="0">VLOOKUP(IF(LOWER(LEFT(E2,9))="reference",LEFT(E2,9),E2),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E2,9))="reference",LEFT(E2,9),E2),Primitive_datatypes,3,FALSE)</f>
+        <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
+This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
+      </c>
+      <c r="G2" s="64" t="s">
+        <v>290</v>
+      </c>
+      <c r="H2" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="65"/>
+    </row>
+    <row r="3" spans="1:13" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="75" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>293</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="63" t="str">
+        <f t="shared" si="0"/>
+        <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
+This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
+      </c>
+      <c r="G3" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="H3" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="65"/>
+    </row>
+    <row r="4" spans="1:13" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="75" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="63" t="str">
+        <f t="shared" si="0"/>
+        <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
+This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
+      </c>
+      <c r="G4" s="64" t="s">
+        <v>235</v>
+      </c>
+      <c r="H4" s="62" t="s">
+        <v>209</v>
+      </c>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="L4" s="63"/>
+      <c r="M4" s="65"/>
+    </row>
+    <row r="5" spans="1:13" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="75" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>296</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="62" t="s">
+        <v>289</v>
+      </c>
+      <c r="F5" s="63" t="str">
+        <f t="shared" si="0"/>
+        <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
+This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
+      </c>
+      <c r="G5" s="66" t="s">
+        <v>297</v>
+      </c>
+      <c r="H5" s="62" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+    </row>
+    <row r="6" spans="1:13" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="75" t="s">
+        <v>298</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>299</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="63" t="str">
+        <f t="shared" ref="F6" si="1">VLOOKUP(IF(LOWER(LEFT(E6,9))="reference",LEFT(E6,9),E6),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E6,9))="reference",LEFT(E6,9),E6),Primitive_datatypes,3,FALSE)</f>
+        <v>A date, or partial date (e.g. just year or year + month) as used in human communication. The format is YYYY, YYYY-MM, or YYYY-MM-DD, e.g. 2018, 1973-06, or 1905-08-23. There SHALL be no time zone. Dates SHALL be valid dates  Regex: ([0-9]([0-9]([0-9][1-9]|[1-9]0)|[1-9]00)|[1-9]000)(-(0[1-9]|1[0-2])(-(0[1-9]|[1-2][0-9]|3[0-1]))?)?</v>
+      </c>
+      <c r="G6" s="66">
+        <v>45303</v>
+      </c>
+      <c r="H6" s="62" t="s">
+        <v>300</v>
+      </c>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+    </row>
+    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="75" t="s">
+        <v>301</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>302</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="62" t="s">
+        <v>254</v>
+      </c>
+      <c r="F7" s="63" t="str">
+        <f t="shared" ref="F7" si="2">VLOOKUP(IF(LOWER(LEFT(E7,9))="reference",LEFT(E7,9),E7),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E7,9))="reference",LEFT(E7,9),E7),Primitive_datatypes,3,FALSE)</f>
+        <v>A signed integer in the range −2,147,483,648..2,147,483,647 (32-bit; for larger values, use decimal)  Regex: [0]|[-+]?[1-9][0-9]*</v>
+      </c>
+      <c r="G7" s="76">
+        <v>12</v>
+      </c>
+      <c r="H7" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+    </row>
+    <row r="8" spans="1:13" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="75" t="s">
+        <v>303</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>304</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>289</v>
+      </c>
+      <c r="F8" s="63" t="str">
+        <f>VLOOKUP(IF(LOWER(LEFT(E8,9))="reference",LEFT(E8,9),E8),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E8,9))="reference",LEFT(E8,9),E8),Primitive_datatypes,3,FALSE)</f>
+        <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
+This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
+      </c>
+      <c r="G8" s="64" t="s">
+        <v>305</v>
+      </c>
+      <c r="H8" s="77" t="s">
+        <v>306</v>
+      </c>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+    </row>
+    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="75" t="s">
+        <v>307</v>
+      </c>
+      <c r="B9" s="62" t="s">
+        <v>308</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="62" t="s">
+        <v>254</v>
+      </c>
+      <c r="F9" s="63" t="str">
+        <f>VLOOKUP(IF(LOWER(LEFT(E9,9))="reference",LEFT(E9,9),E9),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E9,9))="reference",LEFT(E9,9),E9),Primitive_datatypes,3,FALSE)</f>
+        <v>A signed integer in the range −2,147,483,648..2,147,483,647 (32-bit; for larger values, use decimal)  Regex: [0]|[-+]?[1-9][0-9]*</v>
+      </c>
+      <c r="G9" s="64">
+        <v>123</v>
+      </c>
+      <c r="H9" s="62" t="s">
+        <v>309</v>
+      </c>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+    </row>
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="75" t="s">
+        <v>310</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>311</v>
+      </c>
+      <c r="C10" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="78">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E10" s="62" t="s">
+        <v>254</v>
+      </c>
+      <c r="F10" s="63" t="str">
+        <f>VLOOKUP(IF(LOWER(LEFT(E10,9))="reference",LEFT(E10,9),E10),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E10,9))="reference",LEFT(E10,9),E10),Primitive_datatypes,3,FALSE)</f>
+        <v>A signed integer in the range −2,147,483,648..2,147,483,647 (32-bit; for larger values, use decimal)  Regex: [0]|[-+]?[1-9][0-9]*</v>
+      </c>
+      <c r="G10" s="79">
+        <v>1</v>
+      </c>
+      <c r="H10" s="62" t="s">
+        <v>312</v>
+      </c>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1" location="table" tooltip="Minimum and Maximum # of times the the element can appear in the instance" display="http://hl7.org/fhir/R4/formats.html - table" xr:uid="{B83132B4-EE84-4455-ABAB-03E12FBE9B1F}"/>
+    <hyperlink ref="K4" r:id="rId2" xr:uid="{54CCE478-89FB-4D7A-B9CB-9BE58A8E1A86}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB3FC3C-8AAD-41A9-8B0E-ECFDFD4CF5A9}">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="13.05078125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.47265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.3125" customWidth="1"/>
+    <col min="4" max="4" width="4.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.20703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.3671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.47265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.83984375" customWidth="1"/>
+    <col min="9" max="9" width="5.47265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.62890625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.15625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="60" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>345</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="80" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>316</v>
+      </c>
+      <c r="G2" s="81" t="s">
+        <v>317</v>
+      </c>
+      <c r="H2" s="82" t="s">
+        <v>314</v>
+      </c>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>293</v>
+      </c>
+      <c r="C3" s="80" t="s">
+        <v>345</v>
+      </c>
+      <c r="D3" s="81" t="s">
+        <v>318</v>
+      </c>
+      <c r="E3" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>319</v>
+      </c>
+      <c r="G3" s="81" t="s">
+        <v>320</v>
+      </c>
+      <c r="H3" s="82" t="s">
+        <v>292</v>
+      </c>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" s="80" t="s">
+        <v>345</v>
+      </c>
+      <c r="D4" s="83" t="s">
+        <v>318</v>
+      </c>
+      <c r="E4" s="80" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="84" t="s">
+        <v>322</v>
+      </c>
+      <c r="G4" s="83" t="s">
+        <v>323</v>
+      </c>
+      <c r="H4" s="83" t="s">
+        <v>209</v>
+      </c>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="87"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" s="80" t="s">
+        <v>345</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E5" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="75" t="s">
+        <v>327</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C6" s="80" t="s">
+        <v>345</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E6" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="75" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" s="80" t="s">
+        <v>345</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E7" s="80" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="75" t="s">
+        <v>334</v>
+      </c>
+      <c r="B8" s="75" t="s">
+        <v>335</v>
+      </c>
+      <c r="C8" s="80" t="s">
+        <v>345</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E8" s="80" t="s">
+        <v>336</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="75" t="s">
+        <v>338</v>
+      </c>
+      <c r="B9" s="75" t="s">
+        <v>339</v>
+      </c>
+      <c r="C9" s="80" t="s">
+        <v>345</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E9" s="80" t="s">
+        <v>336</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="75" t="s">
+        <v>341</v>
+      </c>
+      <c r="B10" s="75" t="s">
+        <v>342</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>345</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E10" s="80" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="H10" s="75" t="s">
+        <v>341</v>
+      </c>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" location="code" display="code" xr:uid="{6EBA3FDA-A5AA-400E-9646-B5CAFD569C28}"/>
+    <hyperlink ref="D1" r:id="rId2" location="table" tooltip="Minimum and Maximum # of times the the element can appear in the instance" display="http://hl7.org/fhir/R4/formats.html - table" xr:uid="{492259B4-6146-4F9A-AF66-6B196F44A979}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4779,7 +5714,7 @@
       <c r="J2" s="53"/>
       <c r="K2" s="53"/>
       <c r="L2" s="53"/>
-      <c r="M2" s="65" t="s">
+      <c r="M2" s="72" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4814,7 +5749,7 @@
       <c r="J3" s="53"/>
       <c r="K3" s="53"/>
       <c r="L3" s="53"/>
-      <c r="M3" s="66"/>
+      <c r="M3" s="73"/>
     </row>
     <row r="4" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="52" t="s">
@@ -4849,7 +5784,7 @@
         <v>151</v>
       </c>
       <c r="L4" s="53"/>
-      <c r="M4" s="67"/>
+      <c r="M4" s="74"/>
     </row>
     <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="52" t="s">
@@ -5457,439 +6392,439 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="68" t="s">
+      <c r="L1" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="M1" s="68" t="s">
+      <c r="M1" s="60" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="70" t="s">
+      <c r="E2" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="F2" s="71" t="str">
+      <c r="F2" s="63" t="str">
         <f>VLOOKUP(IF(LOWER(LEFT(E2,9))="reference",LEFT(E2,9),E2),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E2,9))="reference",LEFT(E2,9),E2),Primitive_datatypes,3,FALSE)</f>
         <v>A signed integer in the range −2,147,483,648..2,147,483,647 (32-bit; for larger values, use decimal)  Regex: [0]|[-+]?[1-9][0-9]*</v>
       </c>
-      <c r="G2" s="72">
+      <c r="G2" s="64">
         <v>123</v>
       </c>
-      <c r="H2" s="70" t="s">
+      <c r="H2" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71" t="s">
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="M2" s="71"/>
+      <c r="M2" s="63"/>
     </row>
     <row r="3" spans="1:13" ht="114.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="62" t="s">
         <v>208</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="62" t="s">
         <v>224</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="71" t="str">
+      <c r="F3" s="63" t="str">
         <f t="shared" ref="F3:F7" si="0">VLOOKUP(IF(LOWER(LEFT(E3,9))="reference",LEFT(E3,9),E3),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E3,9))="reference",LEFT(E3,9),E3),Primitive_datatypes,3,FALSE)</f>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="64" t="s">
         <v>242</v>
       </c>
-      <c r="H3" s="70" t="s">
+      <c r="H3" s="62" t="s">
         <v>208</v>
       </c>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="73"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="65"/>
     </row>
     <row r="4" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="71" t="str">
+      <c r="F4" s="63" t="str">
         <f t="shared" si="0"/>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G4" s="72" t="s">
+      <c r="G4" s="64" t="s">
         <v>250</v>
       </c>
-      <c r="H4" s="70" t="s">
+      <c r="H4" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="73"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="65"/>
     </row>
     <row r="5" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="62" t="s">
         <v>153</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="62" t="s">
         <v>217</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="70" t="s">
+      <c r="E5" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F5" s="71" t="str">
+      <c r="F5" s="63" t="str">
         <f t="shared" si="0"/>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G5" s="72">
+      <c r="G5" s="64">
         <v>20000</v>
       </c>
-      <c r="H5" s="70" t="s">
+      <c r="H5" s="62" t="s">
         <v>153</v>
       </c>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71" t="s">
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="L5" s="71"/>
-      <c r="M5" s="73"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="65"/>
     </row>
     <row r="6" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="62" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="62" t="s">
         <v>256</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="71" t="str">
+      <c r="F6" s="63" t="str">
         <f t="shared" si="0"/>
         <v>A date, or partial date (e.g. just year or year + month) as used in human communication. The format is YYYY, YYYY-MM, or YYYY-MM-DD, e.g. 2018, 1973-06, or 1905-08-23. There SHALL be no time zone. Dates SHALL be valid dates  Regex: ([0-9]([0-9]([0-9][1-9]|[1-9]0)|[1-9]00)|[1-9]000)(-(0[1-9]|1[0-2])(-(0[1-9]|[1-2][0-9]|3[0-1]))?)?</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="66">
         <v>45303</v>
       </c>
-      <c r="H6" s="70" t="s">
+      <c r="H6" s="62" t="s">
         <v>255</v>
       </c>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
     </row>
     <row r="7" spans="1:13" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="62" t="s">
         <v>258</v>
       </c>
-      <c r="C7" s="70" t="s">
+      <c r="C7" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E7" s="70" t="s">
+      <c r="E7" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F7" s="71" t="str">
+      <c r="F7" s="63" t="str">
         <f t="shared" si="0"/>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G7" s="72">
+      <c r="G7" s="64">
         <v>123</v>
       </c>
-      <c r="H7" s="70" t="s">
+      <c r="H7" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
     </row>
     <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="62" t="s">
         <v>259</v>
       </c>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="62" t="s">
         <v>260</v>
       </c>
-      <c r="C8" s="70" t="s">
+      <c r="C8" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E8" s="70" t="s">
+      <c r="E8" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="F8" s="71" t="str">
+      <c r="F8" s="63" t="str">
         <f>VLOOKUP(IF(LOWER(LEFT(E8,9))="reference",LEFT(E8,9),E8),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E8,9))="reference",LEFT(E8,9),E8),Primitive_datatypes,3,FALSE)</f>
         <v>A signed integer in the range −2,147,483,648..2,147,483,647 (32-bit; for larger values, use decimal)  Regex: [0]|[-+]?[1-9][0-9]*</v>
       </c>
-      <c r="G8" s="72">
+      <c r="G8" s="64">
         <v>123</v>
       </c>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="62" t="s">
         <v>259</v>
       </c>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
     </row>
     <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="62" t="s">
         <v>261</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="62" t="s">
         <v>263</v>
       </c>
-      <c r="C9" s="70" t="s">
+      <c r="C9" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E9" s="70" t="s">
+      <c r="E9" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="F9" s="71" t="str">
+      <c r="F9" s="63" t="str">
         <f>VLOOKUP(IF(LOWER(LEFT(E9,9))="reference",LEFT(E9,9),E9),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E9,9))="reference",LEFT(E9,9),E9),Primitive_datatypes,3,FALSE)</f>
         <v>A signed integer in the range −2,147,483,648..2,147,483,647 (32-bit; for larger values, use decimal)  Regex: [0]|[-+]?[1-9][0-9]*</v>
       </c>
-      <c r="G9" s="72">
+      <c r="G9" s="64">
         <v>123</v>
       </c>
-      <c r="H9" s="70" t="s">
+      <c r="H9" s="62" t="s">
         <v>261</v>
       </c>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="71"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
     </row>
     <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="70" t="s">
+      <c r="A10" s="62" t="s">
         <v>262</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="62" t="s">
         <v>264</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="C10" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E10" s="70" t="s">
+      <c r="E10" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="F10" s="71" t="str">
+      <c r="F10" s="63" t="str">
         <f>VLOOKUP(IF(LOWER(LEFT(E10,9))="reference",LEFT(E10,9),E10),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E10,9))="reference",LEFT(E10,9),E10),Primitive_datatypes,3,FALSE)</f>
         <v>A signed integer in the range −2,147,483,648..2,147,483,647 (32-bit; for larger values, use decimal)  Regex: [0]|[-+]?[1-9][0-9]*</v>
       </c>
-      <c r="G10" s="72">
+      <c r="G10" s="64">
         <v>123</v>
       </c>
-      <c r="H10" s="70" t="s">
+      <c r="H10" s="62" t="s">
         <v>262</v>
       </c>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="71"/>
-      <c r="L10" s="71"/>
-      <c r="M10" s="71"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
     </row>
     <row r="11" spans="1:13" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="62" t="s">
         <v>265</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="62" t="s">
         <v>266</v>
       </c>
-      <c r="C11" s="70" t="s">
+      <c r="C11" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="70" t="s">
+      <c r="E11" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F11" s="71" t="str">
+      <c r="F11" s="63" t="str">
         <f t="shared" ref="F11:F13" si="1">VLOOKUP(IF(LOWER(LEFT(E11,9))="reference",LEFT(E11,9),E11),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E11,9))="reference",LEFT(E11,9),E11),Primitive_datatypes,3,FALSE)</f>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G11" s="72">
+      <c r="G11" s="64">
         <v>123</v>
       </c>
-      <c r="H11" s="70" t="s">
+      <c r="H11" s="62" t="s">
         <v>265</v>
       </c>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="71"/>
-      <c r="M11" s="71"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
     </row>
     <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="62" t="s">
         <v>267</v>
       </c>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="62" t="s">
         <v>268</v>
       </c>
-      <c r="C12" s="70" t="s">
+      <c r="C12" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="E12" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="F12" s="71" t="str">
+      <c r="F12" s="63" t="str">
         <f>VLOOKUP(IF(LOWER(LEFT(E12,9))="reference",LEFT(E12,9),E12),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E12,9))="reference",LEFT(E12,9),E12),Primitive_datatypes,3,FALSE)</f>
         <v>A signed integer in the range −2,147,483,648..2,147,483,647 (32-bit; for larger values, use decimal)  Regex: [0]|[-+]?[1-9][0-9]*</v>
       </c>
-      <c r="G12" s="72">
+      <c r="G12" s="64">
         <v>123</v>
       </c>
-      <c r="H12" s="70" t="s">
+      <c r="H12" s="62" t="s">
         <v>267</v>
       </c>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
     </row>
     <row r="13" spans="1:13" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="62" t="s">
         <v>269</v>
       </c>
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="62" t="s">
         <v>269</v>
       </c>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E13" s="70" t="s">
+      <c r="E13" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F13" s="71" t="str">
+      <c r="F13" s="63" t="str">
         <f t="shared" si="1"/>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G13" s="72">
+      <c r="G13" s="64">
         <v>768.5</v>
       </c>
-      <c r="H13" s="70" t="s">
+      <c r="H13" s="62" t="s">
         <v>269</v>
       </c>
-      <c r="I13" s="71"/>
-      <c r="J13" s="71"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="71"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5928,306 +6863,306 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="68" t="s">
+      <c r="L1" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="M1" s="68" t="s">
+      <c r="M1" s="60" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="114.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="62" t="s">
         <v>208</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="62" t="s">
         <v>224</v>
       </c>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="70" t="s">
+      <c r="E2" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="71" t="str">
+      <c r="F2" s="63" t="str">
         <f t="shared" ref="F2:F5" si="0">VLOOKUP(IF(LOWER(LEFT(E2,9))="reference",LEFT(E2,9),E2),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E2,9))="reference",LEFT(E2,9),E2),Primitive_datatypes,3,FALSE)</f>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G2" s="72" t="s">
+      <c r="G2" s="64" t="s">
         <v>242</v>
       </c>
-      <c r="H2" s="70" t="s">
+      <c r="H2" s="62" t="s">
         <v>208</v>
       </c>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="73"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="65"/>
     </row>
     <row r="3" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="71" t="str">
+      <c r="F3" s="63" t="str">
         <f t="shared" si="0"/>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="64" t="s">
         <v>250</v>
       </c>
-      <c r="H3" s="70" t="s">
+      <c r="H3" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="73"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="65"/>
     </row>
     <row r="4" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="62" t="s">
         <v>153</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="62" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="71" t="str">
+      <c r="F4" s="63" t="str">
         <f t="shared" si="0"/>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G4" s="72">
+      <c r="G4" s="64">
         <v>20000</v>
       </c>
-      <c r="H4" s="70" t="s">
+      <c r="H4" s="62" t="s">
         <v>153</v>
       </c>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71" t="s">
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="L4" s="71"/>
-      <c r="M4" s="73"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="65"/>
     </row>
     <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="62" t="s">
         <v>210</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="62" t="s">
         <v>218</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="70" t="s">
+      <c r="E5" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="71" t="str">
+      <c r="F5" s="63" t="str">
         <f t="shared" si="0"/>
         <v>A date, or partial date (e.g. just year or year + month) as used in human communication. The format is YYYY, YYYY-MM, or YYYY-MM-DD, e.g. 2018, 1973-06, or 1905-08-23. There SHALL be no time zone. Dates SHALL be valid dates  Regex: ([0-9]([0-9]([0-9][1-9]|[1-9]0)|[1-9]00)|[1-9]000)(-(0[1-9]|1[0-2])(-(0[1-9]|[1-2][0-9]|3[0-1]))?)?</v>
       </c>
-      <c r="G5" s="74">
+      <c r="G5" s="66">
         <v>45303</v>
       </c>
-      <c r="H5" s="70" t="s">
+      <c r="H5" s="62" t="s">
         <v>210</v>
       </c>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
     </row>
     <row r="6" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="62" t="s">
         <v>270</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="62" t="s">
         <v>271</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="71" t="str">
+      <c r="F6" s="63" t="str">
         <f t="shared" ref="F6" si="1">VLOOKUP(IF(LOWER(LEFT(E6,9))="reference",LEFT(E6,9),E6),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E6,9))="reference",LEFT(E6,9),E6),Primitive_datatypes,3,FALSE)</f>
         <v>A date, or partial date (e.g. just year or year + month) as used in human communication. The format is YYYY, YYYY-MM, or YYYY-MM-DD, e.g. 2018, 1973-06, or 1905-08-23. There SHALL be no time zone. Dates SHALL be valid dates  Regex: ([0-9]([0-9]([0-9][1-9]|[1-9]0)|[1-9]00)|[1-9]000)(-(0[1-9]|1[0-2])(-(0[1-9]|[1-2][0-9]|3[0-1]))?)?</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="66">
         <v>45303</v>
       </c>
-      <c r="H6" s="70" t="s">
+      <c r="H6" s="62" t="s">
         <v>270</v>
       </c>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
     </row>
     <row r="7" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="62" t="s">
         <v>272</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="62" t="s">
         <v>273</v>
       </c>
-      <c r="C7" s="70" t="s">
+      <c r="C7" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E7" s="70" t="s">
+      <c r="E7" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="71" t="str">
+      <c r="F7" s="63" t="str">
         <f t="shared" ref="F7" si="2">VLOOKUP(IF(LOWER(LEFT(E7,9))="reference",LEFT(E7,9),E7),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E7,9))="reference",LEFT(E7,9),E7),Primitive_datatypes,3,FALSE)</f>
         <v>A date, or partial date (e.g. just year or year + month) as used in human communication. The format is YYYY, YYYY-MM, or YYYY-MM-DD, e.g. 2018, 1973-06, or 1905-08-23. There SHALL be no time zone. Dates SHALL be valid dates  Regex: ([0-9]([0-9]([0-9][1-9]|[1-9]0)|[1-9]00)|[1-9]000)(-(0[1-9]|1[0-2])(-(0[1-9]|[1-2][0-9]|3[0-1]))?)?</v>
       </c>
-      <c r="G7" s="74">
+      <c r="G7" s="66">
         <v>45303</v>
       </c>
-      <c r="H7" s="70" t="s">
+      <c r="H7" s="62" t="s">
         <v>272</v>
       </c>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
     </row>
     <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="62" t="s">
         <v>274</v>
       </c>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="62" t="s">
         <v>275</v>
       </c>
-      <c r="C8" s="70" t="s">
+      <c r="C8" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E8" s="70" t="s">
+      <c r="E8" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="F8" s="71" t="str">
+      <c r="F8" s="63" t="str">
         <f>VLOOKUP(IF(LOWER(LEFT(E8,9))="reference",LEFT(E8,9),E8),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E8,9))="reference",LEFT(E8,9),E8),Primitive_datatypes,3,FALSE)</f>
         <v>A signed integer in the range −2,147,483,648..2,147,483,647 (32-bit; for larger values, use decimal)  Regex: [0]|[-+]?[1-9][0-9]*</v>
       </c>
-      <c r="G8" s="72">
+      <c r="G8" s="64">
         <v>123</v>
       </c>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="62" t="s">
         <v>274</v>
       </c>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
     </row>
     <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="62" t="s">
         <v>276</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="62" t="s">
         <v>277</v>
       </c>
-      <c r="C9" s="70" t="s">
+      <c r="C9" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E9" s="70" t="s">
+      <c r="E9" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="F9" s="71" t="str">
+      <c r="F9" s="63" t="str">
         <f>VLOOKUP(IF(LOWER(LEFT(E9,9))="reference",LEFT(E9,9),E9),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E9,9))="reference",LEFT(E9,9),E9),Primitive_datatypes,3,FALSE)</f>
         <v>A signed integer in the range −2,147,483,648..2,147,483,647 (32-bit; for larger values, use decimal)  Regex: [0]|[-+]?[1-9][0-9]*</v>
       </c>
-      <c r="G9" s="72">
+      <c r="G9" s="64">
         <v>123</v>
       </c>
-      <c r="H9" s="70" t="s">
+      <c r="H9" s="62" t="s">
         <v>276</v>
       </c>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="71"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6266,277 +7201,277 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="68" t="s">
+      <c r="L1" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="M1" s="68" t="s">
+      <c r="M1" s="60" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="114.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="62" t="s">
         <v>208</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="62" t="s">
         <v>224</v>
       </c>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="70" t="s">
+      <c r="E2" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="71" t="str">
+      <c r="F2" s="63" t="str">
         <f t="shared" ref="F2:F7" si="0">VLOOKUP(IF(LOWER(LEFT(E2,9))="reference",LEFT(E2,9),E2),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E2,9))="reference",LEFT(E2,9),E2),Primitive_datatypes,3,FALSE)</f>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G2" s="72" t="s">
+      <c r="G2" s="64" t="s">
         <v>242</v>
       </c>
-      <c r="H2" s="70" t="s">
+      <c r="H2" s="62" t="s">
         <v>208</v>
       </c>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="73"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="65"/>
     </row>
     <row r="3" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="71" t="str">
+      <c r="F3" s="63" t="str">
         <f t="shared" si="0"/>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="64" t="s">
         <v>250</v>
       </c>
-      <c r="H3" s="70" t="s">
+      <c r="H3" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="73"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="65"/>
     </row>
     <row r="4" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="62" t="s">
         <v>278</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="62" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="71" t="str">
+      <c r="F4" s="63" t="str">
         <f t="shared" si="0"/>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G4" s="72">
+      <c r="G4" s="64">
         <v>20000</v>
       </c>
-      <c r="H4" s="70" t="s">
+      <c r="H4" s="62" t="s">
         <v>278</v>
       </c>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71" t="s">
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="L4" s="71"/>
-      <c r="M4" s="73"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="65"/>
     </row>
     <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="62" t="s">
         <v>279</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="62" t="s">
         <v>283</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="70" t="s">
+      <c r="E5" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F5" s="71" t="str">
+      <c r="F5" s="63" t="str">
         <f t="shared" si="0"/>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G5" s="74">
+      <c r="G5" s="66">
         <v>45303</v>
       </c>
-      <c r="H5" s="70" t="s">
+      <c r="H5" s="62" t="s">
         <v>279</v>
       </c>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
     </row>
     <row r="6" spans="1:13" ht="107.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="62" t="s">
         <v>280</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="62" t="s">
         <v>285</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="71" t="str">
+      <c r="F6" s="63" t="str">
         <f t="shared" si="0"/>
         <v>A date, or partial date (e.g. just year or year + month) as used in human communication. The format is YYYY, YYYY-MM, or YYYY-MM-DD, e.g. 2018, 1973-06, or 1905-08-23. There SHALL be no time zone. Dates SHALL be valid dates  Regex: ([0-9]([0-9]([0-9][1-9]|[1-9]0)|[1-9]00)|[1-9]000)(-(0[1-9]|1[0-2])(-(0[1-9]|[1-2][0-9]|3[0-1]))?)?</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="66">
         <v>45527</v>
       </c>
-      <c r="H6" s="70" t="s">
+      <c r="H6" s="62" t="s">
         <v>280</v>
       </c>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
     </row>
     <row r="7" spans="1:13" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="62" t="s">
         <v>281</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="62" t="s">
         <v>284</v>
       </c>
-      <c r="C7" s="70" t="s">
+      <c r="C7" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E7" s="70" t="s">
+      <c r="E7" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F7" s="71" t="str">
+      <c r="F7" s="63" t="str">
         <f t="shared" si="0"/>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G7" s="72" t="s">
+      <c r="G7" s="64" t="s">
         <v>286</v>
       </c>
-      <c r="H7" s="70" t="s">
+      <c r="H7" s="62" t="s">
         <v>281</v>
       </c>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
     </row>
     <row r="8" spans="1:13" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="62" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="62" t="s">
         <v>282</v>
       </c>
-      <c r="C8" s="70" t="s">
+      <c r="C8" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E8" s="70" t="s">
+      <c r="E8" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="71" t="str">
+      <c r="F8" s="63" t="str">
         <f t="shared" ref="F8" si="1">VLOOKUP(IF(LOWER(LEFT(E8,9))="reference",LEFT(E8,9),E8),Primitive_datatypes,2,)&amp;"  "&amp;VLOOKUP(IF(LOWER(LEFT(E8,9))="reference",LEFT(E8,9),E8),Primitive_datatypes,3,FALSE)</f>
         <v>A sequence of Unicode characters. Note that strings SHALL NOT exceed 1MB (1024*1024 characters) in size. Strings SHOULD not contain Unicode character points below 32, except for u0009 (horizontal tab), u0010 (carriage return) and u0013 (line feed). Leading and Trailing whitespace is allowed, but SHOULD be removed when using the XML format. Note: This means that a string that consists only of whitespace could be trimmed to nothing, which would be treated as an invalid element value. Therefore strings SHOULD always contain non-whitespace content.
 This data type can be bound to a ValueSet.  Regex: [ \r\n\t\S]+ (see notes below)</v>
       </c>
-      <c r="G8" s="72" t="s">
+      <c r="G8" s="64" t="s">
         <v>286</v>
       </c>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="62" t="s">
         <v>282</v>
       </c>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6549,15 +7484,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="eaabd3e7-0ce8-42bc-8d66-c3c3304c2dfc">
@@ -6574,6 +7500,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6788,19 +7723,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F3EF619-D41E-4705-9CA4-A271305D0F0D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{209C933E-2063-4D4C-8812-09EB74513F28}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eaabd3e7-0ce8-42bc-8d66-c3c3304c2dfc"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{209C933E-2063-4D4C-8812-09EB74513F28}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F3EF619-D41E-4705-9CA4-A271305D0F0D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="eaabd3e7-0ce8-42bc-8d66-c3c3304c2dfc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>